<commit_message>
[master] update doc/group1.xlsx file
</commit_message>
<xml_diff>
--- a/doc/group1.xlsx
+++ b/doc/group1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15915" windowHeight="7965" tabRatio="1000" activeTab="1"/>
+    <workbookView windowWidth="15915" windowHeight="7965" tabRatio="1000" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Head" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="258">
   <si>
     <t>システム名</t>
   </si>
@@ -568,6 +568,27 @@
     <t>to submit homework</t>
   </si>
   <si>
+    <t>Completed icon</t>
+  </si>
+  <si>
+    <t>assignment complete status</t>
+  </si>
+  <si>
+    <t>Progress icon</t>
+  </si>
+  <si>
+    <t>assignment progess status</t>
+  </si>
+  <si>
+    <t>Lock icon</t>
+  </si>
+  <si>
+    <t>Accordian</t>
+  </si>
+  <si>
+    <t>to view assignment details</t>
+  </si>
+  <si>
     <t>■Homework</t>
   </si>
   <si>
@@ -619,7 +640,7 @@
     <t>AddAComment</t>
   </si>
   <si>
-    <t>SendIcon</t>
+    <t>Send icon</t>
   </si>
   <si>
     <t>to add message</t>
@@ -900,10 +921,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -981,38 +1002,9 @@
       <charset val="128"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1026,11 +1018,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1041,25 +1047,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1074,6 +1071,50 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
@@ -1082,7 +1123,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1102,29 +1143,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1208,79 +1229,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1298,18 +1247,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1317,6 +1254,72 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,19 +1337,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1358,19 +1361,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1382,7 +1403,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1528,6 +1549,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1539,6 +1593,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1560,39 +1638,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1601,181 +1646,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2085,18 +2106,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="8" fillId="0" borderId="12" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="8" fillId="0" borderId="1" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="8" fillId="0" borderId="10" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="8" fillId="0" borderId="3" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="8" fillId="0" borderId="11" xfId="33" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="33" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -18590,342 +18599,342 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="131"/>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="137"/>
+      <c r="A1" s="127"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="133"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="133"/>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="138"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="134"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="133"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="138"/>
+      <c r="A3" s="129"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="134"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="133"/>
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="138"/>
+      <c r="A4" s="129"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="134"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="133"/>
-      <c r="B5" s="134"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="138"/>
+      <c r="A5" s="129"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="130"/>
+      <c r="K5" s="134"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="133"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="138"/>
+      <c r="A6" s="129"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="134"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="133"/>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="138"/>
+      <c r="A7" s="129"/>
+      <c r="B7" s="130"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="134"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="138"/>
+      <c r="A8" s="129"/>
+      <c r="B8" s="130"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="130"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="134"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="133"/>
-      <c r="B9" s="134"/>
-      <c r="C9" s="134"/>
-      <c r="D9" s="134"/>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="134"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="134"/>
-      <c r="K9" s="138"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="130"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="130"/>
+      <c r="G9" s="130"/>
+      <c r="H9" s="130"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
+      <c r="K9" s="134"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="133"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
-      <c r="K10" s="138"/>
+      <c r="A10" s="129"/>
+      <c r="B10" s="130"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="130"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="134"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="133"/>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="134"/>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="138"/>
+      <c r="A11" s="129"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="134"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="133"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="134"/>
-      <c r="K12" s="138"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="134"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="133"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="134"/>
-      <c r="H13" s="134"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="134"/>
-      <c r="K13" s="138"/>
+      <c r="A13" s="129"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="134"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="133"/>
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="134"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="134"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="138"/>
+      <c r="A14" s="129"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="134"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="133"/>
-      <c r="B15" s="134"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
-      <c r="F15" s="134"/>
-      <c r="G15" s="134"/>
-      <c r="H15" s="134"/>
-      <c r="I15" s="134"/>
-      <c r="J15" s="134"/>
-      <c r="K15" s="138"/>
+      <c r="A15" s="129"/>
+      <c r="B15" s="130"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="134"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="133"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="134"/>
-      <c r="I16" s="134"/>
-      <c r="J16" s="134"/>
-      <c r="K16" s="138"/>
+      <c r="A16" s="129"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="130"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="130"/>
+      <c r="I16" s="130"/>
+      <c r="J16" s="130"/>
+      <c r="K16" s="134"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="133"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="134"/>
-      <c r="H17" s="134"/>
-      <c r="I17" s="134"/>
-      <c r="J17" s="134"/>
-      <c r="K17" s="138"/>
+      <c r="A17" s="129"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="130"/>
+      <c r="K17" s="134"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="133"/>
-      <c r="B18" s="134"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="134"/>
-      <c r="K18" s="138"/>
+      <c r="A18" s="129"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="130"/>
+      <c r="I18" s="130"/>
+      <c r="J18" s="130"/>
+      <c r="K18" s="134"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="133"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="134"/>
-      <c r="J19" s="134"/>
-      <c r="K19" s="138"/>
+      <c r="A19" s="129"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="130"/>
+      <c r="H19" s="130"/>
+      <c r="I19" s="130"/>
+      <c r="J19" s="130"/>
+      <c r="K19" s="134"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="133"/>
-      <c r="B20" s="134"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
-      <c r="K20" s="138"/>
+      <c r="A20" s="129"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="130"/>
+      <c r="J20" s="130"/>
+      <c r="K20" s="134"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="133"/>
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="134"/>
-      <c r="I21" s="134"/>
-      <c r="J21" s="134"/>
-      <c r="K21" s="138"/>
+      <c r="A21" s="129"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="130"/>
+      <c r="H21" s="130"/>
+      <c r="I21" s="130"/>
+      <c r="J21" s="130"/>
+      <c r="K21" s="134"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="133"/>
-      <c r="B22" s="134"/>
-      <c r="C22" s="134"/>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="134"/>
-      <c r="I22" s="134"/>
-      <c r="J22" s="134"/>
-      <c r="K22" s="138"/>
+      <c r="A22" s="129"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="130"/>
+      <c r="I22" s="130"/>
+      <c r="J22" s="130"/>
+      <c r="K22" s="134"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="133"/>
-      <c r="B23" s="134"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="134"/>
-      <c r="I23" s="134"/>
-      <c r="J23" s="134"/>
-      <c r="K23" s="138"/>
+      <c r="A23" s="129"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
+      <c r="K23" s="134"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="133"/>
-      <c r="B24" s="134"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="134"/>
-      <c r="I24" s="134"/>
-      <c r="J24" s="134"/>
-      <c r="K24" s="138"/>
+      <c r="A24" s="129"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="130"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="130"/>
+      <c r="I24" s="130"/>
+      <c r="J24" s="130"/>
+      <c r="K24" s="134"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="133"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="134"/>
-      <c r="I25" s="134"/>
-      <c r="J25" s="134"/>
-      <c r="K25" s="138"/>
+      <c r="A25" s="129"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+      <c r="K25" s="134"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="135"/>
-      <c r="B26" s="136"/>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="136"/>
-      <c r="G26" s="136"/>
-      <c r="H26" s="136"/>
-      <c r="I26" s="136"/>
-      <c r="J26" s="136"/>
-      <c r="K26" s="139"/>
+      <c r="A26" s="131"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="132"/>
+      <c r="G26" s="132"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="132"/>
+      <c r="J26" s="132"/>
+      <c r="K26" s="135"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18940,7 +18949,7 @@
   <sheetPr/>
   <dimension ref="B1:BB57"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C43" workbookViewId="0">
       <selection activeCell="K1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
@@ -18948,7 +18957,7 @@
   <sheetData>
     <row r="1" s="60" customFormat="1" ht="13.15" customHeight="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -19198,7 +19207,7 @@
       <c r="Y52" s="62"/>
       <c r="Z52" s="63"/>
       <c r="AA52" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AB52" s="66"/>
       <c r="AC52" s="66"/>
@@ -19267,7 +19276,7 @@
       <c r="Y53" s="62"/>
       <c r="Z53" s="63"/>
       <c r="AA53" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AB53" s="66"/>
       <c r="AC53" s="66"/>
@@ -19336,7 +19345,7 @@
       <c r="Y54" s="62"/>
       <c r="Z54" s="63"/>
       <c r="AA54" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AB54" s="66"/>
       <c r="AC54" s="66"/>
@@ -19353,7 +19362,7 @@
       <c r="AL54" s="78"/>
       <c r="AM54" s="78"/>
       <c r="AN54" s="45" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="AO54" s="45"/>
       <c r="AP54" s="45"/>
@@ -19405,7 +19414,7 @@
       <c r="Y55" s="62"/>
       <c r="Z55" s="63"/>
       <c r="AA55" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AB55" s="66"/>
       <c r="AC55" s="66"/>
@@ -19445,7 +19454,7 @@
       </c>
       <c r="E56" s="63"/>
       <c r="F56" s="15" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="G56" s="64"/>
       <c r="H56" s="64"/>
@@ -19474,7 +19483,7 @@
       <c r="Y56" s="62"/>
       <c r="Z56" s="63"/>
       <c r="AA56" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AB56" s="66"/>
       <c r="AC56" s="66"/>
@@ -19543,7 +19552,7 @@
       <c r="Y57" s="62"/>
       <c r="Z57" s="63"/>
       <c r="AA57" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AB57" s="66"/>
       <c r="AC57" s="66"/>
@@ -19704,7 +19713,7 @@
   <sheetPr/>
   <dimension ref="B1:BD53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="AC53" sqref="AC53:AG53"/>
     </sheetView>
   </sheetViews>
@@ -19726,7 +19735,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -19978,7 +19987,7 @@
       <c r="AA49" s="62"/>
       <c r="AB49" s="63"/>
       <c r="AC49" s="62" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="AD49" s="66"/>
       <c r="AE49" s="66"/>
@@ -20018,7 +20027,7 @@
       </c>
       <c r="G50" s="63"/>
       <c r="H50" s="15" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="I50" s="64"/>
       <c r="J50" s="64"/>
@@ -20047,7 +20056,7 @@
       <c r="AA50" s="62"/>
       <c r="AB50" s="63"/>
       <c r="AC50" s="62" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="AD50" s="66"/>
       <c r="AE50" s="66"/>
@@ -20087,7 +20096,7 @@
       </c>
       <c r="G51" s="63"/>
       <c r="H51" s="15" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="I51" s="64"/>
       <c r="J51" s="64"/>
@@ -20116,7 +20125,7 @@
       <c r="AA51" s="62"/>
       <c r="AB51" s="63"/>
       <c r="AC51" s="62" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="AD51" s="66"/>
       <c r="AE51" s="66"/>
@@ -20152,7 +20161,7 @@
       </c>
       <c r="G52" s="63"/>
       <c r="H52" s="15" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="I52" s="64"/>
       <c r="J52" s="64"/>
@@ -20179,7 +20188,7 @@
       <c r="AA52" s="62"/>
       <c r="AB52" s="63"/>
       <c r="AC52" s="62" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="AD52" s="66"/>
       <c r="AE52" s="66"/>
@@ -20215,7 +20224,7 @@
       </c>
       <c r="G53" s="63"/>
       <c r="H53" s="15" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="I53" s="64"/>
       <c r="J53" s="64"/>
@@ -20240,7 +20249,7 @@
       <c r="AA53" s="62"/>
       <c r="AB53" s="63"/>
       <c r="AC53" s="62" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="AD53" s="66"/>
       <c r="AE53" s="66"/>
@@ -20384,7 +20393,7 @@
   <sheetPr/>
   <dimension ref="B1:BD84"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="AW84" sqref="AW84:BD84"/>
     </sheetView>
   </sheetViews>
@@ -20404,7 +20413,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -20656,7 +20665,7 @@
       <c r="AA72" s="62"/>
       <c r="AB72" s="63"/>
       <c r="AC72" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD72" s="66"/>
       <c r="AE72" s="66"/>
@@ -20696,7 +20705,7 @@
       </c>
       <c r="G73" s="63"/>
       <c r="H73" s="15" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="I73" s="64"/>
       <c r="J73" s="64"/>
@@ -20725,7 +20734,7 @@
       <c r="AA73" s="62"/>
       <c r="AB73" s="63"/>
       <c r="AC73" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD73" s="66"/>
       <c r="AE73" s="66"/>
@@ -20794,7 +20803,7 @@
       <c r="AA74" s="62"/>
       <c r="AB74" s="63"/>
       <c r="AC74" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD74" s="66"/>
       <c r="AE74" s="66"/>
@@ -20811,7 +20820,7 @@
       <c r="AN74" s="78"/>
       <c r="AO74" s="78"/>
       <c r="AP74" s="45" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="AQ74" s="45"/>
       <c r="AR74" s="45"/>
@@ -20863,7 +20872,7 @@
       <c r="AA75" s="62"/>
       <c r="AB75" s="63"/>
       <c r="AC75" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD75" s="66"/>
       <c r="AE75" s="66"/>
@@ -20903,7 +20912,7 @@
       </c>
       <c r="G76" s="63"/>
       <c r="H76" s="15" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="I76" s="64"/>
       <c r="J76" s="64"/>
@@ -20932,7 +20941,7 @@
       <c r="AA76" s="62"/>
       <c r="AB76" s="63"/>
       <c r="AC76" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD76" s="66"/>
       <c r="AE76" s="66"/>
@@ -20949,7 +20958,7 @@
       <c r="AN76" s="78"/>
       <c r="AO76" s="78"/>
       <c r="AP76" s="45" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="AQ76" s="45"/>
       <c r="AR76" s="45"/>
@@ -21001,7 +21010,7 @@
       <c r="AA77" s="62"/>
       <c r="AB77" s="63"/>
       <c r="AC77" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD77" s="66"/>
       <c r="AE77" s="66"/>
@@ -21070,7 +21079,7 @@
       <c r="AA78" s="62"/>
       <c r="AB78" s="63"/>
       <c r="AC78" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD78" s="66"/>
       <c r="AE78" s="66"/>
@@ -21110,7 +21119,7 @@
       </c>
       <c r="G79" s="63"/>
       <c r="H79" s="15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="I79" s="64"/>
       <c r="J79" s="64"/>
@@ -21139,7 +21148,7 @@
       <c r="AA79" s="62"/>
       <c r="AB79" s="63"/>
       <c r="AC79" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD79" s="66"/>
       <c r="AE79" s="66"/>
@@ -21175,7 +21184,7 @@
       </c>
       <c r="G80" s="63"/>
       <c r="H80" s="15" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="I80" s="64"/>
       <c r="J80" s="64"/>
@@ -21204,7 +21213,7 @@
       <c r="AA80" s="62"/>
       <c r="AB80" s="63"/>
       <c r="AC80" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD80" s="66"/>
       <c r="AE80" s="66"/>
@@ -21273,7 +21282,7 @@
       <c r="AA81" s="62"/>
       <c r="AB81" s="63"/>
       <c r="AC81" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD81" s="66"/>
       <c r="AE81" s="66"/>
@@ -21313,7 +21322,7 @@
       </c>
       <c r="G82" s="63"/>
       <c r="H82" s="15" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I82" s="64"/>
       <c r="J82" s="64"/>
@@ -21340,7 +21349,7 @@
       <c r="AA82" s="62"/>
       <c r="AB82" s="63"/>
       <c r="AC82" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD82" s="66"/>
       <c r="AE82" s="66"/>
@@ -21376,7 +21385,7 @@
       </c>
       <c r="G83" s="63"/>
       <c r="H83" s="15" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="I83" s="64"/>
       <c r="J83" s="64"/>
@@ -21435,7 +21444,7 @@
       </c>
       <c r="G84" s="63"/>
       <c r="H84" s="15" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="I84" s="64"/>
       <c r="J84" s="64"/>
@@ -21462,7 +21471,7 @@
       <c r="AA84" s="62"/>
       <c r="AB84" s="63"/>
       <c r="AC84" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AD84" s="66"/>
       <c r="AE84" s="66"/>
@@ -21484,7 +21493,7 @@
       <c r="AU84" s="45"/>
       <c r="AV84" s="45"/>
       <c r="AW84" s="67" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AX84" s="64"/>
       <c r="AY84" s="64"/>
@@ -21720,7 +21729,7 @@
   <sheetPr/>
   <dimension ref="B1:BA84"/>
   <sheetViews>
-    <sheetView topLeftCell="O64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="AT84" sqref="AT84:BA84"/>
     </sheetView>
   </sheetViews>
@@ -21728,7 +21737,7 @@
   <sheetData>
     <row r="1" s="60" customFormat="1" ht="13.15" customHeight="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -21960,7 +21969,7 @@
       </c>
       <c r="D69" s="63"/>
       <c r="E69" s="15" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="F69" s="64"/>
       <c r="G69" s="64"/>
@@ -22011,7 +22020,7 @@
       <c r="AR69" s="45"/>
       <c r="AS69" s="45"/>
       <c r="AT69" s="67" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AU69" s="64"/>
       <c r="AV69" s="64"/>
@@ -22056,7 +22065,7 @@
       <c r="X70" s="62"/>
       <c r="Y70" s="63"/>
       <c r="Z70" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA70" s="66"/>
       <c r="AB70" s="66"/>
@@ -22096,7 +22105,7 @@
       </c>
       <c r="D71" s="63"/>
       <c r="E71" s="15" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="F71" s="64"/>
       <c r="G71" s="64"/>
@@ -22125,7 +22134,7 @@
       <c r="X71" s="62"/>
       <c r="Y71" s="63"/>
       <c r="Z71" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA71" s="66"/>
       <c r="AB71" s="66"/>
@@ -22194,7 +22203,7 @@
       <c r="X72" s="62"/>
       <c r="Y72" s="63"/>
       <c r="Z72" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA72" s="66"/>
       <c r="AB72" s="66"/>
@@ -22211,7 +22220,7 @@
       <c r="AK72" s="78"/>
       <c r="AL72" s="78"/>
       <c r="AM72" s="45" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="AN72" s="45"/>
       <c r="AO72" s="45"/>
@@ -22263,7 +22272,7 @@
       <c r="X73" s="62"/>
       <c r="Y73" s="63"/>
       <c r="Z73" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA73" s="66"/>
       <c r="AB73" s="66"/>
@@ -22332,7 +22341,7 @@
       <c r="X74" s="62"/>
       <c r="Y74" s="63"/>
       <c r="Z74" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA74" s="66"/>
       <c r="AB74" s="66"/>
@@ -22401,7 +22410,7 @@
       <c r="X75" s="62"/>
       <c r="Y75" s="63"/>
       <c r="Z75" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA75" s="66"/>
       <c r="AB75" s="66"/>
@@ -22441,7 +22450,7 @@
       </c>
       <c r="D76" s="63"/>
       <c r="E76" s="15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F76" s="64"/>
       <c r="G76" s="64"/>
@@ -22470,7 +22479,7 @@
       <c r="X76" s="62"/>
       <c r="Y76" s="63"/>
       <c r="Z76" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA76" s="66"/>
       <c r="AB76" s="66"/>
@@ -22506,7 +22515,7 @@
       </c>
       <c r="D77" s="63"/>
       <c r="E77" s="15" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F77" s="64"/>
       <c r="G77" s="64"/>
@@ -22535,7 +22544,7 @@
       <c r="X77" s="62"/>
       <c r="Y77" s="63"/>
       <c r="Z77" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA77" s="66"/>
       <c r="AB77" s="66"/>
@@ -22604,7 +22613,7 @@
       <c r="X78" s="62"/>
       <c r="Y78" s="63"/>
       <c r="Z78" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA78" s="66"/>
       <c r="AB78" s="66"/>
@@ -22644,7 +22653,7 @@
       </c>
       <c r="D79" s="63"/>
       <c r="E79" s="15" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="F79" s="64"/>
       <c r="G79" s="64"/>
@@ -22671,7 +22680,7 @@
       <c r="X79" s="62"/>
       <c r="Y79" s="63"/>
       <c r="Z79" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA79" s="66"/>
       <c r="AB79" s="66"/>
@@ -22707,7 +22716,7 @@
       </c>
       <c r="D80" s="63"/>
       <c r="E80" s="15" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F80" s="64"/>
       <c r="G80" s="64"/>
@@ -22734,7 +22743,7 @@
       <c r="X80" s="62"/>
       <c r="Y80" s="63"/>
       <c r="Z80" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA80" s="66"/>
       <c r="AB80" s="66"/>
@@ -22770,7 +22779,7 @@
       </c>
       <c r="D81" s="63"/>
       <c r="E81" s="15" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F81" s="64"/>
       <c r="G81" s="64"/>
@@ -22797,7 +22806,7 @@
       <c r="X81" s="62"/>
       <c r="Y81" s="63"/>
       <c r="Z81" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA81" s="66"/>
       <c r="AB81" s="66"/>
@@ -22833,7 +22842,7 @@
       </c>
       <c r="D82" s="63"/>
       <c r="E82" s="15" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="F82" s="64"/>
       <c r="G82" s="64"/>
@@ -22860,7 +22869,7 @@
       <c r="X82" s="62"/>
       <c r="Y82" s="63"/>
       <c r="Z82" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA82" s="66"/>
       <c r="AB82" s="66"/>
@@ -22896,7 +22905,7 @@
       </c>
       <c r="D83" s="63"/>
       <c r="E83" s="15" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="F83" s="64"/>
       <c r="G83" s="64"/>
@@ -22955,7 +22964,7 @@
       </c>
       <c r="D84" s="63"/>
       <c r="E84" s="15" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="F84" s="64"/>
       <c r="G84" s="64"/>
@@ -22982,7 +22991,7 @@
       <c r="X84" s="62"/>
       <c r="Y84" s="63"/>
       <c r="Z84" s="62" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="AA84" s="66"/>
       <c r="AB84" s="66"/>
@@ -23004,7 +23013,7 @@
       <c r="AR84" s="45"/>
       <c r="AS84" s="45"/>
       <c r="AT84" s="67" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AU84" s="64"/>
       <c r="AV84" s="64"/>
@@ -23289,7 +23298,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="2:11">
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -23702,7 +23711,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
@@ -23922,7 +23931,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -24021,7 +24030,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="21"/>
       <c r="L17" s="21" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -24107,7 +24116,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
@@ -24115,7 +24124,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
       <c r="R19" s="28" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="S19" s="29"/>
       <c r="T19" s="29"/>
@@ -24197,7 +24206,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="21"/>
       <c r="L21" s="21" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
@@ -24205,7 +24214,7 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="28" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="S21" s="29"/>
       <c r="T21" s="29"/>
@@ -24287,7 +24296,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
@@ -24295,7 +24304,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
       <c r="R23" s="28" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="S23" s="29"/>
       <c r="T23" s="29"/>
@@ -24908,7 +24917,7 @@
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="15" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
@@ -24967,7 +24976,7 @@
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="15" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
@@ -25007,13 +25016,13 @@
       <c r="AF39" s="44"/>
       <c r="AG39" s="44"/>
       <c r="AH39" s="45" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AI39" s="45"/>
       <c r="AJ39" s="45"/>
       <c r="AK39" s="45"/>
       <c r="AL39" s="45" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="AM39" s="45"/>
       <c r="AN39" s="45"/>
@@ -25057,7 +25066,7 @@
       </c>
       <c r="R40" s="14"/>
       <c r="S40" s="13" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="T40" s="14"/>
       <c r="U40" s="13"/>
@@ -25076,13 +25085,13 @@
       <c r="AF40" s="44"/>
       <c r="AG40" s="44"/>
       <c r="AH40" s="45" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AI40" s="45"/>
       <c r="AJ40" s="45"/>
       <c r="AK40" s="45"/>
       <c r="AL40" s="15" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="AM40" s="16"/>
       <c r="AN40" s="16"/>
@@ -25105,7 +25114,7 @@
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="15" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -25145,13 +25154,13 @@
       <c r="AF41" s="44"/>
       <c r="AG41" s="44"/>
       <c r="AH41" s="45" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AI41" s="45"/>
       <c r="AJ41" s="45"/>
       <c r="AK41" s="45"/>
       <c r="AL41" s="45" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="AM41" s="45"/>
       <c r="AN41" s="45"/>
@@ -25174,7 +25183,7 @@
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="15" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
@@ -25182,7 +25191,7 @@
       <c r="H42" s="16"/>
       <c r="I42" s="24"/>
       <c r="J42" s="15" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="K42" s="16"/>
       <c r="L42" s="16"/>
@@ -25201,7 +25210,7 @@
       <c r="U42" s="13"/>
       <c r="V42" s="14"/>
       <c r="W42" s="13" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="X42" s="14"/>
       <c r="Y42" s="13"/>
@@ -25214,13 +25223,13 @@
       <c r="AF42" s="44"/>
       <c r="AG42" s="44"/>
       <c r="AH42" s="45" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AI42" s="45"/>
       <c r="AJ42" s="45"/>
       <c r="AK42" s="45"/>
       <c r="AL42" s="45" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="AM42" s="45"/>
       <c r="AN42" s="45"/>
@@ -25243,7 +25252,7 @@
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="15" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
@@ -25251,7 +25260,7 @@
       <c r="H43" s="16"/>
       <c r="I43" s="24"/>
       <c r="J43" s="15" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="K43" s="16"/>
       <c r="L43" s="16"/>
@@ -25270,7 +25279,7 @@
       <c r="U43" s="13"/>
       <c r="V43" s="14"/>
       <c r="W43" s="13" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="X43" s="14"/>
       <c r="Y43" s="13"/>
@@ -25283,13 +25292,13 @@
       <c r="AF43" s="44"/>
       <c r="AG43" s="44"/>
       <c r="AH43" s="45" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AI43" s="45"/>
       <c r="AJ43" s="45"/>
       <c r="AK43" s="45"/>
       <c r="AL43" s="45" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="AM43" s="45"/>
       <c r="AN43" s="45"/>
@@ -25312,7 +25321,7 @@
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="15" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
@@ -25320,7 +25329,7 @@
       <c r="H44" s="16"/>
       <c r="I44" s="24"/>
       <c r="J44" s="15" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="K44" s="16"/>
       <c r="L44" s="16"/>
@@ -25339,7 +25348,7 @@
       <c r="U44" s="13"/>
       <c r="V44" s="14"/>
       <c r="W44" s="13" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="X44" s="14"/>
       <c r="Y44" s="13"/>
@@ -25352,13 +25361,13 @@
       <c r="AF44" s="44"/>
       <c r="AG44" s="44"/>
       <c r="AH44" s="45" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="AI44" s="45"/>
       <c r="AJ44" s="45"/>
       <c r="AK44" s="45"/>
       <c r="AL44" s="45" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="AM44" s="45"/>
       <c r="AN44" s="45"/>
@@ -25381,7 +25390,7 @@
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="15" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
@@ -25428,7 +25437,7 @@
       <c r="AQ45" s="45"/>
       <c r="AR45" s="45"/>
       <c r="AS45" s="56" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="AT45" s="57"/>
       <c r="AU45" s="57"/>
@@ -25444,7 +25453,7 @@
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
@@ -25491,7 +25500,7 @@
       <c r="AQ46" s="45"/>
       <c r="AR46" s="45"/>
       <c r="AS46" s="56" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="AT46" s="57"/>
       <c r="AU46" s="57"/>
@@ -25507,7 +25516,7 @@
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="19" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="20"/>
@@ -25515,7 +25524,7 @@
       <c r="H47" s="20"/>
       <c r="I47" s="26"/>
       <c r="J47" s="19" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="K47" s="20"/>
       <c r="L47" s="20"/>
@@ -25554,7 +25563,7 @@
       <c r="AQ47" s="27"/>
       <c r="AR47" s="18"/>
       <c r="AS47" s="17" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="AT47" s="27"/>
       <c r="AU47" s="27"/>
@@ -25727,11 +25736,11 @@
     <mergeCell ref="Q35:R37"/>
   </mergeCells>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q38:R47">
+      <formula1>"I, O"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J38:M46">
       <formula1>"Textbox, File Input, Button, Label, Link"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q38:R47">
-      <formula1>"I, O"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S38:T46">
       <formula1>"〇, ☓"</formula1>
@@ -25749,7 +25758,7 @@
   <sheetPr/>
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -26173,10 +26182,10 @@
       <c r="J17" s="105"/>
       <c r="K17" s="105"/>
       <c r="L17" s="105"/>
-      <c r="M17" s="125">
+      <c r="M17" s="117">
         <v>44507</v>
       </c>
-      <c r="N17" s="126"/>
+      <c r="N17" s="118"/>
       <c r="O17" s="119" t="s">
         <v>35</v>
       </c>
@@ -26201,8 +26210,8 @@
       <c r="J18" s="105"/>
       <c r="K18" s="105"/>
       <c r="L18" s="105"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="128"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="121"/>
       <c r="O18" s="115" t="s">
         <v>26</v>
       </c>
@@ -26227,8 +26236,8 @@
       <c r="J19" s="105"/>
       <c r="K19" s="105"/>
       <c r="L19" s="105"/>
-      <c r="M19" s="127"/>
-      <c r="N19" s="128"/>
+      <c r="M19" s="120"/>
+      <c r="N19" s="121"/>
       <c r="O19" s="115" t="s">
         <v>26</v>
       </c>
@@ -26253,12 +26262,12 @@
       <c r="J20" s="105"/>
       <c r="K20" s="105"/>
       <c r="L20" s="105"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="128"/>
-      <c r="O20" s="129" t="s">
+      <c r="M20" s="120"/>
+      <c r="N20" s="121"/>
+      <c r="O20" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="P20" s="130"/>
+      <c r="P20" s="126"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="109"/>
@@ -28162,7 +28171,7 @@
   <sheetPr/>
   <dimension ref="B1:BD60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="AP55" sqref="AP55:AV55"/>
     </sheetView>
   </sheetViews>
@@ -28912,10 +28921,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:BD66"/>
+  <dimension ref="B1:BD70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A66" sqref="$A66:$XFD66"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="AY73" sqref="AY73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.71428571428571" defaultRowHeight="13.15" customHeight="1"/>
@@ -29927,8 +29936,250 @@
       <c r="BC66" s="64"/>
       <c r="BD66" s="65"/>
     </row>
+    <row r="67" customHeight="1" spans="6:56">
+      <c r="F67" s="62">
+        <v>13</v>
+      </c>
+      <c r="G67" s="63"/>
+      <c r="H67" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="I67" s="64"/>
+      <c r="J67" s="64"/>
+      <c r="K67" s="64"/>
+      <c r="L67" s="64"/>
+      <c r="M67" s="65"/>
+      <c r="N67" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="O67" s="64"/>
+      <c r="P67" s="64"/>
+      <c r="Q67" s="65"/>
+      <c r="R67" s="62"/>
+      <c r="S67" s="66"/>
+      <c r="T67" s="63"/>
+      <c r="U67" s="62"/>
+      <c r="V67" s="63"/>
+      <c r="W67" s="62"/>
+      <c r="X67" s="63"/>
+      <c r="Y67" s="62"/>
+      <c r="Z67" s="63"/>
+      <c r="AA67" s="62"/>
+      <c r="AB67" s="63"/>
+      <c r="AC67" s="62"/>
+      <c r="AD67" s="66"/>
+      <c r="AE67" s="66"/>
+      <c r="AF67" s="66"/>
+      <c r="AG67" s="63"/>
+      <c r="AH67" s="77"/>
+      <c r="AI67" s="77"/>
+      <c r="AJ67" s="77"/>
+      <c r="AK67" s="77"/>
+      <c r="AL67" s="45"/>
+      <c r="AM67" s="45"/>
+      <c r="AN67" s="45"/>
+      <c r="AO67" s="45"/>
+      <c r="AP67" s="45"/>
+      <c r="AQ67" s="45"/>
+      <c r="AR67" s="45"/>
+      <c r="AS67" s="45"/>
+      <c r="AT67" s="45"/>
+      <c r="AU67" s="45"/>
+      <c r="AV67" s="45"/>
+      <c r="AW67" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="AX67" s="64"/>
+      <c r="AY67" s="64"/>
+      <c r="AZ67" s="64"/>
+      <c r="BA67" s="64"/>
+      <c r="BB67" s="64"/>
+      <c r="BC67" s="64"/>
+      <c r="BD67" s="65"/>
+    </row>
+    <row r="68" customHeight="1" spans="6:56">
+      <c r="F68" s="62">
+        <v>14</v>
+      </c>
+      <c r="G68" s="63"/>
+      <c r="H68" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="I68" s="64"/>
+      <c r="J68" s="64"/>
+      <c r="K68" s="64"/>
+      <c r="L68" s="64"/>
+      <c r="M68" s="65"/>
+      <c r="N68" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="O68" s="64"/>
+      <c r="P68" s="64"/>
+      <c r="Q68" s="65"/>
+      <c r="R68" s="62"/>
+      <c r="S68" s="66"/>
+      <c r="T68" s="63"/>
+      <c r="U68" s="62"/>
+      <c r="V68" s="63"/>
+      <c r="W68" s="62"/>
+      <c r="X68" s="63"/>
+      <c r="Y68" s="62"/>
+      <c r="Z68" s="63"/>
+      <c r="AA68" s="62"/>
+      <c r="AB68" s="63"/>
+      <c r="AC68" s="62"/>
+      <c r="AD68" s="66"/>
+      <c r="AE68" s="66"/>
+      <c r="AF68" s="66"/>
+      <c r="AG68" s="63"/>
+      <c r="AH68" s="77"/>
+      <c r="AI68" s="77"/>
+      <c r="AJ68" s="77"/>
+      <c r="AK68" s="77"/>
+      <c r="AL68" s="45"/>
+      <c r="AM68" s="45"/>
+      <c r="AN68" s="45"/>
+      <c r="AO68" s="45"/>
+      <c r="AP68" s="45"/>
+      <c r="AQ68" s="45"/>
+      <c r="AR68" s="45"/>
+      <c r="AS68" s="45"/>
+      <c r="AT68" s="45"/>
+      <c r="AU68" s="45"/>
+      <c r="AV68" s="45"/>
+      <c r="AW68" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX68" s="64"/>
+      <c r="AY68" s="64"/>
+      <c r="AZ68" s="64"/>
+      <c r="BA68" s="64"/>
+      <c r="BB68" s="64"/>
+      <c r="BC68" s="64"/>
+      <c r="BD68" s="65"/>
+    </row>
+    <row r="69" customHeight="1" spans="6:56">
+      <c r="F69" s="62">
+        <v>15</v>
+      </c>
+      <c r="G69" s="63"/>
+      <c r="H69" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="I69" s="64"/>
+      <c r="J69" s="64"/>
+      <c r="K69" s="64"/>
+      <c r="L69" s="64"/>
+      <c r="M69" s="65"/>
+      <c r="N69" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="O69" s="64"/>
+      <c r="P69" s="64"/>
+      <c r="Q69" s="65"/>
+      <c r="R69" s="62"/>
+      <c r="S69" s="66"/>
+      <c r="T69" s="63"/>
+      <c r="U69" s="62"/>
+      <c r="V69" s="63"/>
+      <c r="W69" s="62"/>
+      <c r="X69" s="63"/>
+      <c r="Y69" s="62"/>
+      <c r="Z69" s="63"/>
+      <c r="AA69" s="62"/>
+      <c r="AB69" s="63"/>
+      <c r="AC69" s="62"/>
+      <c r="AD69" s="66"/>
+      <c r="AE69" s="66"/>
+      <c r="AF69" s="66"/>
+      <c r="AG69" s="63"/>
+      <c r="AH69" s="77"/>
+      <c r="AI69" s="77"/>
+      <c r="AJ69" s="77"/>
+      <c r="AK69" s="77"/>
+      <c r="AL69" s="45"/>
+      <c r="AM69" s="45"/>
+      <c r="AN69" s="45"/>
+      <c r="AO69" s="45"/>
+      <c r="AP69" s="45"/>
+      <c r="AQ69" s="45"/>
+      <c r="AR69" s="45"/>
+      <c r="AS69" s="45"/>
+      <c r="AT69" s="45"/>
+      <c r="AU69" s="45"/>
+      <c r="AV69" s="45"/>
+      <c r="AW69" s="67"/>
+      <c r="AX69" s="64"/>
+      <c r="AY69" s="64"/>
+      <c r="AZ69" s="64"/>
+      <c r="BA69" s="64"/>
+      <c r="BB69" s="64"/>
+      <c r="BC69" s="64"/>
+      <c r="BD69" s="65"/>
+    </row>
+    <row r="70" customHeight="1" spans="6:56">
+      <c r="F70" s="62">
+        <v>16</v>
+      </c>
+      <c r="G70" s="63"/>
+      <c r="H70" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="I70" s="64"/>
+      <c r="J70" s="64"/>
+      <c r="K70" s="64"/>
+      <c r="L70" s="64"/>
+      <c r="M70" s="65"/>
+      <c r="N70" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="O70" s="64"/>
+      <c r="P70" s="64"/>
+      <c r="Q70" s="65"/>
+      <c r="R70" s="62"/>
+      <c r="S70" s="66"/>
+      <c r="T70" s="63"/>
+      <c r="U70" s="62"/>
+      <c r="V70" s="63"/>
+      <c r="W70" s="62"/>
+      <c r="X70" s="63"/>
+      <c r="Y70" s="62"/>
+      <c r="Z70" s="63"/>
+      <c r="AA70" s="62"/>
+      <c r="AB70" s="63"/>
+      <c r="AC70" s="62"/>
+      <c r="AD70" s="66"/>
+      <c r="AE70" s="66"/>
+      <c r="AF70" s="66"/>
+      <c r="AG70" s="63"/>
+      <c r="AH70" s="77"/>
+      <c r="AI70" s="77"/>
+      <c r="AJ70" s="77"/>
+      <c r="AK70" s="77"/>
+      <c r="AL70" s="45"/>
+      <c r="AM70" s="45"/>
+      <c r="AN70" s="45"/>
+      <c r="AO70" s="45"/>
+      <c r="AP70" s="45"/>
+      <c r="AQ70" s="45"/>
+      <c r="AR70" s="45"/>
+      <c r="AS70" s="45"/>
+      <c r="AT70" s="45"/>
+      <c r="AU70" s="45"/>
+      <c r="AV70" s="45"/>
+      <c r="AW70" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="AX70" s="64"/>
+      <c r="AY70" s="64"/>
+      <c r="AZ70" s="64"/>
+      <c r="BA70" s="64"/>
+      <c r="BB70" s="64"/>
+      <c r="BC70" s="64"/>
+      <c r="BD70" s="65"/>
+    </row>
   </sheetData>
-  <mergeCells count="186">
+  <mergeCells count="242">
     <mergeCell ref="W52:AB52"/>
     <mergeCell ref="Y53:AB53"/>
     <mergeCell ref="Y54:Z54"/>
@@ -30103,6 +30354,62 @@
     <mergeCell ref="AL66:AO66"/>
     <mergeCell ref="AP66:AV66"/>
     <mergeCell ref="AW66:BD66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:M67"/>
+    <mergeCell ref="N67:Q67"/>
+    <mergeCell ref="R67:T67"/>
+    <mergeCell ref="U67:V67"/>
+    <mergeCell ref="W67:X67"/>
+    <mergeCell ref="Y67:Z67"/>
+    <mergeCell ref="AA67:AB67"/>
+    <mergeCell ref="AC67:AG67"/>
+    <mergeCell ref="AH67:AI67"/>
+    <mergeCell ref="AJ67:AK67"/>
+    <mergeCell ref="AL67:AO67"/>
+    <mergeCell ref="AP67:AV67"/>
+    <mergeCell ref="AW67:BD67"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="H68:M68"/>
+    <mergeCell ref="N68:Q68"/>
+    <mergeCell ref="R68:T68"/>
+    <mergeCell ref="U68:V68"/>
+    <mergeCell ref="W68:X68"/>
+    <mergeCell ref="Y68:Z68"/>
+    <mergeCell ref="AA68:AB68"/>
+    <mergeCell ref="AC68:AG68"/>
+    <mergeCell ref="AH68:AI68"/>
+    <mergeCell ref="AJ68:AK68"/>
+    <mergeCell ref="AL68:AO68"/>
+    <mergeCell ref="AP68:AV68"/>
+    <mergeCell ref="AW68:BD68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:M69"/>
+    <mergeCell ref="N69:Q69"/>
+    <mergeCell ref="R69:T69"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="W69:X69"/>
+    <mergeCell ref="Y69:Z69"/>
+    <mergeCell ref="AA69:AB69"/>
+    <mergeCell ref="AC69:AG69"/>
+    <mergeCell ref="AH69:AI69"/>
+    <mergeCell ref="AJ69:AK69"/>
+    <mergeCell ref="AL69:AO69"/>
+    <mergeCell ref="AP69:AV69"/>
+    <mergeCell ref="AW69:BD69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="H70:M70"/>
+    <mergeCell ref="N70:Q70"/>
+    <mergeCell ref="R70:T70"/>
+    <mergeCell ref="U70:V70"/>
+    <mergeCell ref="W70:X70"/>
+    <mergeCell ref="Y70:Z70"/>
+    <mergeCell ref="AA70:AB70"/>
+    <mergeCell ref="AC70:AG70"/>
+    <mergeCell ref="AH70:AI70"/>
+    <mergeCell ref="AJ70:AK70"/>
+    <mergeCell ref="AL70:AO70"/>
+    <mergeCell ref="AP70:AV70"/>
+    <mergeCell ref="AW70:BD70"/>
     <mergeCell ref="B1:J2"/>
     <mergeCell ref="F52:G54"/>
     <mergeCell ref="AH52:AI54"/>
@@ -30117,13 +30424,13 @@
     <mergeCell ref="W53:X54"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N59:Q59 N60:Q60 N61:Q61 N62:Q62 N63:Q63 N64:Q64 N65:Q65 N66:Q66 N55:Q58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N59:Q59 N60:Q60 N61:Q61 N62:Q62 N63:Q63 N64:Q64 N65:Q65 N66:Q66 N67:Q67 N68:Q68 N69:Q69 N70:Q70 N55:Q58">
       <formula1>"Textbox, Button, Label, Link"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U59:V59 U60:V60 U61:V61 U62:V62 U63:V63 U64:V64 U65:V65 U66:V66 U55:V58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U59:V59 U60:V60 U61:V61 U62:V62 U63:V63 U64:V64 U65:V65 U66:V66 U67:V67 U68:V68 U69:V69 U70:V70 U55:V58">
       <formula1>"I, O"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W59:X59 W60:X60 W61:X61 W62:X62 W63:X63 W64:X64 W65:X65 W66:X66 W55:X58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W59:X59 W60:X60 W61:X61 W62:X62 W63:X63 W64:X64 W65:X65 W66:X66 W67:X67 W68:X68 W69:X69 W70:X70 W55:X58">
       <formula1>"〇, ☓"</formula1>
     </dataValidation>
   </dataValidations>
@@ -30139,7 +30446,7 @@
   <sheetPr/>
   <dimension ref="B1:BD58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -30161,7 +30468,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -30384,7 +30691,7 @@
       </c>
       <c r="G51" s="63"/>
       <c r="H51" s="15" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="I51" s="64"/>
       <c r="J51" s="64"/>
@@ -30431,7 +30738,7 @@
       <c r="AU51" s="78"/>
       <c r="AV51" s="78"/>
       <c r="AW51" s="67" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="AX51" s="64"/>
       <c r="AY51" s="64"/>
@@ -30447,7 +30754,7 @@
       </c>
       <c r="G52" s="63"/>
       <c r="H52" s="15" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="I52" s="64"/>
       <c r="J52" s="64"/>
@@ -30512,7 +30819,7 @@
       </c>
       <c r="G53" s="63"/>
       <c r="H53" s="15" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="I53" s="64"/>
       <c r="J53" s="64"/>
@@ -30585,7 +30892,7 @@
       <c r="L54" s="64"/>
       <c r="M54" s="65"/>
       <c r="N54" s="15" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="O54" s="64"/>
       <c r="P54" s="64"/>
@@ -30707,7 +31014,7 @@
       </c>
       <c r="G56" s="63"/>
       <c r="H56" s="15" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="I56" s="64"/>
       <c r="J56" s="64"/>
@@ -30754,7 +31061,7 @@
       <c r="AU56" s="45"/>
       <c r="AV56" s="45"/>
       <c r="AW56" s="67" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="AX56" s="64"/>
       <c r="AY56" s="64"/>
@@ -30770,7 +31077,7 @@
       </c>
       <c r="G57" s="63"/>
       <c r="H57" s="15" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="I57" s="64"/>
       <c r="J57" s="64"/>
@@ -30833,7 +31140,7 @@
       </c>
       <c r="G58" s="63"/>
       <c r="H58" s="15" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I58" s="64"/>
       <c r="J58" s="64"/>
@@ -31048,8 +31355,8 @@
   <sheetPr/>
   <dimension ref="B1:BD63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63:M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.71428571428571" defaultRowHeight="13.15" customHeight="1"/>
@@ -31070,7 +31377,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -31293,7 +31600,7 @@
       </c>
       <c r="G51" s="63"/>
       <c r="H51" s="15" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="I51" s="64"/>
       <c r="J51" s="64"/>
@@ -31340,7 +31647,7 @@
       <c r="AU51" s="78"/>
       <c r="AV51" s="78"/>
       <c r="AW51" s="67" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="AX51" s="64"/>
       <c r="AY51" s="64"/>
@@ -31356,7 +31663,7 @@
       </c>
       <c r="G52" s="63"/>
       <c r="H52" s="15" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="I52" s="64"/>
       <c r="J52" s="64"/>
@@ -31421,7 +31728,7 @@
       </c>
       <c r="G53" s="63"/>
       <c r="H53" s="15" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="I53" s="64"/>
       <c r="J53" s="64"/>
@@ -31468,7 +31775,7 @@
       <c r="AU53" s="78"/>
       <c r="AV53" s="78"/>
       <c r="AW53" s="67" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="AX53" s="64"/>
       <c r="AY53" s="64"/>
@@ -31484,7 +31791,7 @@
       </c>
       <c r="G54" s="63"/>
       <c r="H54" s="15" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="I54" s="64"/>
       <c r="J54" s="64"/>
@@ -31549,7 +31856,7 @@
       </c>
       <c r="G55" s="63"/>
       <c r="H55" s="15" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="I55" s="64"/>
       <c r="J55" s="64"/>
@@ -31622,7 +31929,7 @@
       <c r="L56" s="64"/>
       <c r="M56" s="65"/>
       <c r="N56" s="15" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="O56" s="64"/>
       <c r="P56" s="64"/>
@@ -31744,7 +32051,7 @@
       </c>
       <c r="G58" s="63"/>
       <c r="H58" s="15" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="I58" s="64"/>
       <c r="J58" s="64"/>
@@ -31771,7 +32078,7 @@
       <c r="AA58" s="62"/>
       <c r="AB58" s="63"/>
       <c r="AC58" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AD58" s="66"/>
       <c r="AE58" s="66"/>
@@ -31793,7 +32100,7 @@
       <c r="AU58" s="45"/>
       <c r="AV58" s="45"/>
       <c r="AW58" s="67" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="AX58" s="64"/>
       <c r="AY58" s="64"/>
@@ -31809,7 +32116,7 @@
       </c>
       <c r="G59" s="63"/>
       <c r="H59" s="15" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="I59" s="64"/>
       <c r="J59" s="64"/>
@@ -31856,7 +32163,7 @@
       <c r="AU59" s="45"/>
       <c r="AV59" s="45"/>
       <c r="AW59" s="67" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="AX59" s="64"/>
       <c r="AY59" s="64"/>
@@ -31872,7 +32179,7 @@
       </c>
       <c r="G60" s="63"/>
       <c r="H60" s="15" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="I60" s="64"/>
       <c r="J60" s="64"/>
@@ -31935,7 +32242,7 @@
       </c>
       <c r="G61" s="63"/>
       <c r="H61" s="15" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I61" s="64"/>
       <c r="J61" s="64"/>
@@ -32000,7 +32307,7 @@
       </c>
       <c r="G62" s="63"/>
       <c r="H62" s="15" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="I62" s="64"/>
       <c r="J62" s="64"/>
@@ -32027,7 +32334,7 @@
       <c r="AA62" s="62"/>
       <c r="AB62" s="63"/>
       <c r="AC62" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AD62" s="66"/>
       <c r="AE62" s="66"/>
@@ -32063,11 +32370,11 @@
     </row>
     <row r="63" customHeight="1" spans="6:56">
       <c r="F63" s="62">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G63" s="63"/>
       <c r="H63" s="15" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="I63" s="64"/>
       <c r="J63" s="64"/>
@@ -32094,7 +32401,7 @@
       <c r="AA63" s="62"/>
       <c r="AB63" s="63"/>
       <c r="AC63" s="62" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AD63" s="66"/>
       <c r="AE63" s="66"/>
@@ -32116,7 +32423,7 @@
       <c r="AU63" s="45"/>
       <c r="AV63" s="45"/>
       <c r="AW63" s="67" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="AX63" s="64"/>
       <c r="AY63" s="64"/>

</xml_diff>